<commit_message>
Added prompt message if user enters incorrect data type into entry box
Added rubrics in Excel file
</commit_message>
<xml_diff>
--- a/ExtractedData.xlsx
+++ b/ExtractedData.xlsx
@@ -8,13 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\MorePycharmProjects\DemandPlanning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A82E776-08E7-457F-877C-6E8BDAE3D3D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{654A6732-8A48-4D58-AFC2-C457D4F386B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{FD45604D-BDDA-4A13-8576-BD85EC70AD81}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{FD45604D-BDDA-4A13-8576-BD85EC70AD81}"/>
   </bookViews>
   <sheets>
-    <sheet name="Assignment" sheetId="2" r:id="rId1"/>
-    <sheet name="Data" sheetId="1" r:id="rId2"/>
+    <sheet name="Data" sheetId="1" r:id="rId1"/>
+    <sheet name="Assignment" sheetId="2" r:id="rId2"/>
+    <sheet name="Rubrics" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -147,10 +148,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
@@ -462,6 +462,109 @@
         </a:p>
       </xdr:txBody>
     </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>37562</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C4EA8288-BFFD-6226-DFF4-A58AAD5E4A96}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="85725" y="200025"/>
+          <a:ext cx="6619875" cy="3647537"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>190501</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>79732</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F52E37FD-7E2B-61A9-8635-7CCFD6E004B7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6896101" y="200025"/>
+          <a:ext cx="6477000" cy="3689707"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:ln w="12700">
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
@@ -783,21 +886,6 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCBABD8D-0962-4669-90DB-85085E16615E}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C36" sqref="C36"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC07FAB6-1418-4446-9941-AEE0A20658FE}">
   <dimension ref="A1:J20"/>
   <sheetViews>
@@ -818,34 +906,34 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="3" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="I1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="J1" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -865,19 +953,19 @@
       <c r="E2" s="1">
         <v>60</v>
       </c>
-      <c r="F2" s="2">
+      <c r="F2" s="1">
         <v>2.99</v>
       </c>
-      <c r="G2" s="4">
+      <c r="G2" s="3">
         <v>1</v>
       </c>
-      <c r="H2" s="2">
+      <c r="H2" s="1">
         <v>219.08</v>
       </c>
-      <c r="I2" s="2">
+      <c r="I2" s="1">
         <v>112.14</v>
       </c>
-      <c r="J2" s="2">
+      <c r="J2" s="1">
         <v>108.08</v>
       </c>
     </row>
@@ -897,19 +985,19 @@
       <c r="E3" s="1">
         <v>60</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="1">
         <v>4.51</v>
       </c>
-      <c r="G3" s="4">
+      <c r="G3" s="3">
         <v>0.98</v>
       </c>
-      <c r="H3" s="2">
+      <c r="H3" s="1">
         <v>172.88</v>
       </c>
-      <c r="I3" s="2">
+      <c r="I3" s="1">
         <v>58.56</v>
       </c>
-      <c r="J3" s="2">
+      <c r="J3" s="1">
         <v>116.56</v>
       </c>
     </row>
@@ -929,19 +1017,19 @@
       <c r="E4" s="1">
         <v>60</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="1">
         <v>4.87</v>
       </c>
-      <c r="G4" s="4">
+      <c r="G4" s="3">
         <v>0.92</v>
       </c>
-      <c r="H4" s="2">
+      <c r="H4" s="1">
         <v>181.3</v>
       </c>
-      <c r="I4" s="2">
+      <c r="I4" s="1">
         <v>63.3</v>
       </c>
-      <c r="J4" s="2">
+      <c r="J4" s="1">
         <v>119.84</v>
       </c>
     </row>
@@ -961,19 +1049,19 @@
       <c r="E5" s="1">
         <v>60</v>
       </c>
-      <c r="F5" s="2">
+      <c r="F5" s="1">
         <v>4.87</v>
       </c>
-      <c r="G5" s="4">
+      <c r="G5" s="3">
         <v>0.92</v>
       </c>
-      <c r="H5" s="2">
+      <c r="H5" s="1">
         <v>181.24</v>
       </c>
-      <c r="I5" s="2">
+      <c r="I5" s="1">
         <v>63.18</v>
       </c>
-      <c r="J5" s="2">
+      <c r="J5" s="1">
         <v>119.9</v>
       </c>
     </row>
@@ -993,51 +1081,51 @@
       <c r="E6" s="1">
         <v>60</v>
       </c>
-      <c r="F6" s="2">
+      <c r="F6" s="1">
         <v>3.86</v>
       </c>
-      <c r="G6" s="4">
+      <c r="G6" s="3">
         <v>0.99</v>
       </c>
-      <c r="H6" s="2">
+      <c r="H6" s="1">
         <v>206.98</v>
       </c>
-      <c r="I6" s="2">
+      <c r="I6" s="1">
         <v>90.48</v>
       </c>
-      <c r="J6" s="2">
+      <c r="J6" s="1">
         <v>118.04</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+      <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G8" s="3" t="s">
+      <c r="G8" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="H8" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I8" s="3" t="s">
+      <c r="I8" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J8" s="3" t="s">
+      <c r="J8" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1057,19 +1145,19 @@
       <c r="E9" s="1">
         <v>150</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="1">
         <v>2.84</v>
       </c>
-      <c r="G9" s="4">
+      <c r="G9" s="3">
         <v>1</v>
       </c>
-      <c r="H9" s="2">
+      <c r="H9" s="1">
         <v>260.92</v>
       </c>
-      <c r="I9" s="2">
+      <c r="I9" s="1">
         <v>134.63999999999999</v>
       </c>
-      <c r="J9" s="2">
+      <c r="J9" s="1">
         <v>126.08</v>
       </c>
     </row>
@@ -1089,19 +1177,19 @@
       <c r="E10" s="1">
         <v>150</v>
       </c>
-      <c r="F10" s="2">
+      <c r="F10" s="1">
         <v>2.74</v>
       </c>
-      <c r="G10" s="4">
+      <c r="G10" s="3">
         <v>1</v>
       </c>
-      <c r="H10" s="2">
+      <c r="H10" s="1">
         <v>263.08</v>
       </c>
-      <c r="I10" s="2">
+      <c r="I10" s="1">
         <v>137.58000000000001</v>
       </c>
-      <c r="J10" s="2">
+      <c r="J10" s="1">
         <v>124.98</v>
       </c>
     </row>
@@ -1121,19 +1209,19 @@
       <c r="E11" s="1">
         <v>150</v>
       </c>
-      <c r="F11" s="2">
+      <c r="F11" s="1">
         <v>3.67</v>
       </c>
-      <c r="G11" s="4">
+      <c r="G11" s="3">
         <v>0.99</v>
       </c>
-      <c r="H11" s="2">
+      <c r="H11" s="1">
         <v>247.06</v>
       </c>
-      <c r="I11" s="2">
+      <c r="I11" s="1">
         <v>105.2</v>
       </c>
-      <c r="J11" s="2">
+      <c r="J11" s="1">
         <v>141.74</v>
       </c>
     </row>
@@ -1153,19 +1241,19 @@
       <c r="E12" s="1">
         <v>150</v>
       </c>
-      <c r="F12" s="2">
+      <c r="F12" s="1">
         <v>4.37</v>
       </c>
-      <c r="G12" s="4">
+      <c r="G12" s="3">
         <v>0.93</v>
       </c>
-      <c r="H12" s="2">
+      <c r="H12" s="1">
         <v>250.38</v>
       </c>
-      <c r="I12" s="2">
+      <c r="I12" s="1">
         <v>78.84</v>
       </c>
-      <c r="J12" s="2">
+      <c r="J12" s="1">
         <v>171.08</v>
       </c>
     </row>
@@ -1185,51 +1273,51 @@
       <c r="E13" s="1">
         <v>150</v>
       </c>
-      <c r="F13" s="2">
+      <c r="F13" s="1">
         <v>4.5999999999999996</v>
       </c>
-      <c r="G13" s="4">
+      <c r="G13" s="3">
         <v>0.9</v>
       </c>
-      <c r="H13" s="2">
+      <c r="H13" s="1">
         <v>247.2</v>
       </c>
-      <c r="I13" s="2">
+      <c r="I13" s="1">
         <v>74.959999999999994</v>
       </c>
-      <c r="J13" s="2">
+      <c r="J13" s="1">
         <v>171.44</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C15" s="3" t="s">
+      <c r="C15" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D15" s="3" t="s">
+      <c r="D15" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E15" s="3" t="s">
+      <c r="E15" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F15" s="3" t="s">
+      <c r="F15" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G15" s="3" t="s">
+      <c r="G15" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H15" s="3" t="s">
+      <c r="H15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I15" s="3" t="s">
+      <c r="I15" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J15" s="3" t="s">
+      <c r="J15" s="2" t="s">
         <v>9</v>
       </c>
     </row>
@@ -1249,19 +1337,19 @@
       <c r="E16" s="1">
         <v>250</v>
       </c>
-      <c r="F16" s="2">
+      <c r="F16" s="1">
         <v>2.61</v>
       </c>
-      <c r="G16" s="4">
+      <c r="G16" s="3">
         <v>1</v>
       </c>
-      <c r="H16" s="2">
+      <c r="H16" s="1">
         <v>311.38</v>
       </c>
-      <c r="I16" s="2">
+      <c r="I16" s="1">
         <v>186.84</v>
       </c>
-      <c r="J16" s="2">
+      <c r="J16" s="1">
         <v>125.34</v>
       </c>
     </row>
@@ -1281,19 +1369,19 @@
       <c r="E17" s="1">
         <v>250</v>
       </c>
-      <c r="F17" s="2">
+      <c r="F17" s="1">
         <v>2.48</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>1</v>
       </c>
-      <c r="H17" s="2">
+      <c r="H17" s="1">
         <v>298.86</v>
       </c>
-      <c r="I17" s="2">
+      <c r="I17" s="1">
         <v>174.14</v>
       </c>
-      <c r="J17" s="2">
+      <c r="J17" s="1">
         <v>124.34</v>
       </c>
     </row>
@@ -1313,19 +1401,19 @@
       <c r="E18" s="1">
         <v>250</v>
       </c>
-      <c r="F18" s="2">
+      <c r="F18" s="1">
         <v>2.34</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>1</v>
       </c>
-      <c r="H18" s="2">
+      <c r="H18" s="1">
         <v>308.06</v>
       </c>
-      <c r="I18" s="2">
+      <c r="I18" s="1">
         <v>184.5</v>
       </c>
-      <c r="J18" s="2">
+      <c r="J18" s="1">
         <v>122.86</v>
       </c>
     </row>
@@ -1345,19 +1433,19 @@
       <c r="E19" s="1">
         <v>250</v>
       </c>
-      <c r="F19" s="2">
+      <c r="F19" s="1">
         <v>3.07</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>0.98</v>
       </c>
-      <c r="H19" s="2">
+      <c r="H19" s="1">
         <v>294.82</v>
       </c>
-      <c r="I19" s="2">
+      <c r="I19" s="1">
         <v>155.62</v>
       </c>
-      <c r="J19" s="2">
+      <c r="J19" s="1">
         <v>136.9</v>
       </c>
     </row>
@@ -1377,19 +1465,19 @@
       <c r="E20" s="1">
         <v>250</v>
       </c>
-      <c r="F20" s="2">
+      <c r="F20" s="1">
         <v>3.86</v>
       </c>
-      <c r="G20" s="4">
+      <c r="G20" s="3">
         <v>0.95</v>
       </c>
-      <c r="H20" s="2">
+      <c r="H20" s="1">
         <v>283.52</v>
       </c>
-      <c r="I20" s="2">
+      <c r="I20" s="1">
         <v>117.12</v>
       </c>
-      <c r="J20" s="2">
+      <c r="J20" s="1">
         <v>166.96</v>
       </c>
     </row>
@@ -1397,4 +1485,34 @@
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BCBABD8D-0962-4669-90DB-85085E16615E}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BEDB73EC-A4BB-42C3-9BAA-01FA76380362}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Y11" sqref="Y11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>